<commit_message>
Add tests from another source and make change one case
</commit_message>
<xml_diff>
--- a/ExchangeRates.xlsx
+++ b/ExchangeRates.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Desktop\finance\tax\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Desktop\finance\tax_calc\tax\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="ExchangeRates" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <t>בנק ישראל - שערים יציגים</t>
   </si>
   <si>
-    <t>טווח תאריכים : 02/01/2019 - 07/06/2019</t>
+    <t>טווח תאריכים : 02/01/2019 - 28/06/2019</t>
   </si>
   <si>
     <t>אם לא פורסם שער יציג ליום המבוקש, מוצג השער האחרון שפורסם לפניו</t>
@@ -908,9 +908,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B110"/>
+  <dimension ref="A1:B125"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1781,6 +1783,126 @@
         <v>3.601</v>
       </c>
     </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="4">
+        <v>43626</v>
+      </c>
+      <c r="B111" s="5">
+        <v>3.585</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="4">
+        <v>43627</v>
+      </c>
+      <c r="B112" s="5">
+        <v>3.581</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="4">
+        <v>43628</v>
+      </c>
+      <c r="B113" s="5">
+        <v>3.5819999999999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="4">
+        <v>43629</v>
+      </c>
+      <c r="B114" s="5">
+        <v>3.5920000000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="4">
+        <v>43630</v>
+      </c>
+      <c r="B115" s="5">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="4">
+        <v>43633</v>
+      </c>
+      <c r="B116" s="5">
+        <v>3.61</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="4">
+        <v>43634</v>
+      </c>
+      <c r="B117" s="5">
+        <v>3.6120000000000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="4">
+        <v>43635</v>
+      </c>
+      <c r="B118" s="5">
+        <v>3.609</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="4">
+        <v>43636</v>
+      </c>
+      <c r="B119" s="5">
+        <v>3.5790000000000002</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="4">
+        <v>43637</v>
+      </c>
+      <c r="B120" s="5">
+        <v>3.5939999999999999</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="4">
+        <v>43640</v>
+      </c>
+      <c r="B121" s="5">
+        <v>3.6040000000000001</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="4">
+        <v>43641</v>
+      </c>
+      <c r="B122" s="5">
+        <v>3.6019999999999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="4">
+        <v>43642</v>
+      </c>
+      <c r="B123" s="5">
+        <v>3.5910000000000002</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="4">
+        <v>43643</v>
+      </c>
+      <c r="B124" s="5">
+        <v>3.5819999999999999</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="4">
+        <v>43644</v>
+      </c>
+      <c r="B125" s="5">
+        <v>3.5659999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Get exchage rates dynamically from bank of Israel site
</commit_message>
<xml_diff>
--- a/ExchangeRates.xlsx
+++ b/ExchangeRates.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="ExchangeRates" sheetId="1" r:id="rId1"/>
+    <sheet name="ExchangeRates (4)" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -24,7 +24,7 @@
     <t>בנק ישראל - שערים יציגים</t>
   </si>
   <si>
-    <t>טווח תאריכים : 02/01/2019 - 28/06/2019</t>
+    <t>טווח תאריכים : 02/01/2019 - 20/12/2019</t>
   </si>
   <si>
     <t>אם לא פורסם שער יציג ליום המבוקש, מוצג השער האחרון שפורסם לפניו</t>
@@ -908,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B125"/>
+  <dimension ref="A1:B243"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1903,8 +1903,952 @@
         <v>3.5659999999999998</v>
       </c>
     </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="4">
+        <v>43647</v>
+      </c>
+      <c r="B126" s="5">
+        <v>3.5739999999999998</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="4">
+        <v>43648</v>
+      </c>
+      <c r="B127" s="5">
+        <v>3.5750000000000002</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="4">
+        <v>43649</v>
+      </c>
+      <c r="B128" s="5">
+        <v>3.5720000000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="4">
+        <v>43650</v>
+      </c>
+      <c r="B129" s="5">
+        <v>3.5670000000000002</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="4">
+        <v>43651</v>
+      </c>
+      <c r="B130" s="5">
+        <v>3.5619999999999998</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="4">
+        <v>43654</v>
+      </c>
+      <c r="B131" s="5">
+        <v>3.573</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="4">
+        <v>43655</v>
+      </c>
+      <c r="B132" s="5">
+        <v>3.5680000000000001</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="4">
+        <v>43656</v>
+      </c>
+      <c r="B133" s="5">
+        <v>3.573</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="4">
+        <v>43657</v>
+      </c>
+      <c r="B134" s="5">
+        <v>3.5470000000000002</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="4">
+        <v>43658</v>
+      </c>
+      <c r="B135" s="5">
+        <v>3.5510000000000002</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="4">
+        <v>43661</v>
+      </c>
+      <c r="B136" s="5">
+        <v>3.5390000000000001</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="4">
+        <v>43662</v>
+      </c>
+      <c r="B137" s="5">
+        <v>3.5419999999999998</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="4">
+        <v>43663</v>
+      </c>
+      <c r="B138" s="5">
+        <v>3.5409999999999999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="4">
+        <v>43664</v>
+      </c>
+      <c r="B139" s="5">
+        <v>3.5430000000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="4">
+        <v>43665</v>
+      </c>
+      <c r="B140" s="5">
+        <v>3.5350000000000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="4">
+        <v>43668</v>
+      </c>
+      <c r="B141" s="5">
+        <v>3.5339999999999998</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="4">
+        <v>43669</v>
+      </c>
+      <c r="B142" s="5">
+        <v>3.5369999999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="4">
+        <v>43670</v>
+      </c>
+      <c r="B143" s="5">
+        <v>3.5209999999999999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="4">
+        <v>43671</v>
+      </c>
+      <c r="B144" s="5">
+        <v>3.5230000000000001</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="4">
+        <v>43672</v>
+      </c>
+      <c r="B145" s="5">
+        <v>3.5259999999999998</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="4">
+        <v>43675</v>
+      </c>
+      <c r="B146" s="5">
+        <v>3.5249999999999999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="4">
+        <v>43676</v>
+      </c>
+      <c r="B147" s="5">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="4">
+        <v>43677</v>
+      </c>
+      <c r="B148" s="5">
+        <v>3.4990000000000001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="4">
+        <v>43678</v>
+      </c>
+      <c r="B149" s="5">
+        <v>3.524</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="4">
+        <v>43679</v>
+      </c>
+      <c r="B150" s="5">
+        <v>3.5089999999999999</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="4">
+        <v>43682</v>
+      </c>
+      <c r="B151" s="5">
+        <v>3.4940000000000002</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="4">
+        <v>43683</v>
+      </c>
+      <c r="B152" s="5">
+        <v>3.4940000000000002</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="4">
+        <v>43684</v>
+      </c>
+      <c r="B153" s="5">
+        <v>3.4870000000000001</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="4">
+        <v>43685</v>
+      </c>
+      <c r="B154" s="5">
+        <v>3.4830000000000001</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="4">
+        <v>43686</v>
+      </c>
+      <c r="B155" s="5">
+        <v>3.4790000000000001</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="4">
+        <v>43689</v>
+      </c>
+      <c r="B156" s="5">
+        <v>3.484</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="4">
+        <v>43690</v>
+      </c>
+      <c r="B157" s="5">
+        <v>3.4929999999999999</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="4">
+        <v>43691</v>
+      </c>
+      <c r="B158" s="5">
+        <v>3.4889999999999999</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="4">
+        <v>43692</v>
+      </c>
+      <c r="B159" s="5">
+        <v>3.5190000000000001</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="4">
+        <v>43693</v>
+      </c>
+      <c r="B160" s="5">
+        <v>3.5409999999999999</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="4">
+        <v>43696</v>
+      </c>
+      <c r="B161" s="5">
+        <v>3.5449999999999999</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="4">
+        <v>43697</v>
+      </c>
+      <c r="B162" s="5">
+        <v>3.524</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="4">
+        <v>43698</v>
+      </c>
+      <c r="B163" s="5">
+        <v>3.5270000000000001</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="4">
+        <v>43699</v>
+      </c>
+      <c r="B164" s="5">
+        <v>3.5249999999999999</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="4">
+        <v>43700</v>
+      </c>
+      <c r="B165" s="5">
+        <v>3.5110000000000001</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="4">
+        <v>43703</v>
+      </c>
+      <c r="B166" s="5">
+        <v>3.5190000000000001</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="4">
+        <v>43704</v>
+      </c>
+      <c r="B167" s="5">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="4">
+        <v>43705</v>
+      </c>
+      <c r="B168" s="5">
+        <v>3.524</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="4">
+        <v>43706</v>
+      </c>
+      <c r="B169" s="5">
+        <v>3.5209999999999999</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="4">
+        <v>43707</v>
+      </c>
+      <c r="B170" s="5">
+        <v>3.5350000000000001</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="4">
+        <v>43710</v>
+      </c>
+      <c r="B171" s="5">
+        <v>3.5379999999999998</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="4">
+        <v>43711</v>
+      </c>
+      <c r="B172" s="5">
+        <v>3.5489999999999999</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="4">
+        <v>43712</v>
+      </c>
+      <c r="B173" s="5">
+        <v>3.5270000000000001</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="4">
+        <v>43713</v>
+      </c>
+      <c r="B174" s="5">
+        <v>3.512</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" s="4">
+        <v>43714</v>
+      </c>
+      <c r="B175" s="5">
+        <v>3.5169999999999999</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="4">
+        <v>43717</v>
+      </c>
+      <c r="B176" s="5">
+        <v>3.5270000000000001</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="4">
+        <v>43718</v>
+      </c>
+      <c r="B177" s="5">
+        <v>3.5379999999999998</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="4">
+        <v>43719</v>
+      </c>
+      <c r="B178" s="5">
+        <v>3.544</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="4">
+        <v>43720</v>
+      </c>
+      <c r="B179" s="5">
+        <v>3.5409999999999999</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="4">
+        <v>43721</v>
+      </c>
+      <c r="B180" s="5">
+        <v>3.5270000000000001</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="4">
+        <v>43724</v>
+      </c>
+      <c r="B181" s="5">
+        <v>3.5379999999999998</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="4">
+        <v>43726</v>
+      </c>
+      <c r="B182" s="5">
+        <v>3.5409999999999999</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" s="4">
+        <v>43727</v>
+      </c>
+      <c r="B183" s="5">
+        <v>3.5209999999999999</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" s="4">
+        <v>43728</v>
+      </c>
+      <c r="B184" s="5">
+        <v>3.5129999999999999</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" s="4">
+        <v>43731</v>
+      </c>
+      <c r="B185" s="5">
+        <v>3.5169999999999999</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" s="4">
+        <v>43732</v>
+      </c>
+      <c r="B186" s="5">
+        <v>3.5070000000000001</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" s="4">
+        <v>43733</v>
+      </c>
+      <c r="B187" s="5">
+        <v>3.5009999999999999</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" s="4">
+        <v>43734</v>
+      </c>
+      <c r="B188" s="5">
+        <v>3.5169999999999999</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" s="4">
+        <v>43735</v>
+      </c>
+      <c r="B189" s="5">
+        <v>3.4820000000000002</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" s="4">
+        <v>43740</v>
+      </c>
+      <c r="B190" s="5">
+        <v>3.4849999999999999</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" s="4">
+        <v>43741</v>
+      </c>
+      <c r="B191" s="5">
+        <v>3.4929999999999999</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" s="4">
+        <v>43742</v>
+      </c>
+      <c r="B192" s="5">
+        <v>3.4809999999999999</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" s="4">
+        <v>43745</v>
+      </c>
+      <c r="B193" s="5">
+        <v>3.4929999999999999</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" s="4">
+        <v>43748</v>
+      </c>
+      <c r="B194" s="5">
+        <v>3.504</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" s="4">
+        <v>43749</v>
+      </c>
+      <c r="B195" s="5">
+        <v>3.51</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" s="4">
+        <v>43753</v>
+      </c>
+      <c r="B196" s="5">
+        <v>3.5129999999999999</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" s="4">
+        <v>43754</v>
+      </c>
+      <c r="B197" s="5">
+        <v>3.536</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" s="4">
+        <v>43755</v>
+      </c>
+      <c r="B198" s="5">
+        <v>3.5449999999999999</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" s="4">
+        <v>43756</v>
+      </c>
+      <c r="B199" s="5">
+        <v>3.5329999999999999</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" s="4">
+        <v>43760</v>
+      </c>
+      <c r="B200" s="5">
+        <v>3.5369999999999999</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" s="4">
+        <v>43761</v>
+      </c>
+      <c r="B201" s="5">
+        <v>3.5379999999999998</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" s="4">
+        <v>43762</v>
+      </c>
+      <c r="B202" s="5">
+        <v>3.5230000000000001</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" s="4">
+        <v>43763</v>
+      </c>
+      <c r="B203" s="5">
+        <v>3.5390000000000001</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" s="4">
+        <v>43766</v>
+      </c>
+      <c r="B204" s="5">
+        <v>3.5289999999999999</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" s="4">
+        <v>43767</v>
+      </c>
+      <c r="B205" s="5">
+        <v>3.53</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206" s="4">
+        <v>43768</v>
+      </c>
+      <c r="B206" s="5">
+        <v>3.528</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207" s="4">
+        <v>43769</v>
+      </c>
+      <c r="B207" s="5">
+        <v>3.5289999999999999</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208" s="4">
+        <v>43770</v>
+      </c>
+      <c r="B208" s="5">
+        <v>3.5209999999999999</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" s="4">
+        <v>43773</v>
+      </c>
+      <c r="B209" s="5">
+        <v>3.5219999999999998</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" s="4">
+        <v>43774</v>
+      </c>
+      <c r="B210" s="5">
+        <v>3.5009999999999999</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211" s="4">
+        <v>43775</v>
+      </c>
+      <c r="B211" s="5">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212" s="4">
+        <v>43776</v>
+      </c>
+      <c r="B212" s="5">
+        <v>3.4870000000000001</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213" s="4">
+        <v>43777</v>
+      </c>
+      <c r="B213" s="5">
+        <v>3.4950000000000001</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214" s="4">
+        <v>43780</v>
+      </c>
+      <c r="B214" s="5">
+        <v>3.4990000000000001</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215" s="4">
+        <v>43781</v>
+      </c>
+      <c r="B215" s="5">
+        <v>3.5110000000000001</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216" s="4">
+        <v>43782</v>
+      </c>
+      <c r="B216" s="5">
+        <v>3.4950000000000001</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217" s="4">
+        <v>43783</v>
+      </c>
+      <c r="B217" s="5">
+        <v>3.488</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218" s="4">
+        <v>43784</v>
+      </c>
+      <c r="B218" s="5">
+        <v>3.4780000000000002</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219" s="4">
+        <v>43787</v>
+      </c>
+      <c r="B219" s="5">
+        <v>3.4630000000000001</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220" s="4">
+        <v>43788</v>
+      </c>
+      <c r="B220" s="5">
+        <v>3.4569999999999999</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221" s="4">
+        <v>43789</v>
+      </c>
+      <c r="B221" s="5">
+        <v>3.4710000000000001</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222" s="4">
+        <v>43790</v>
+      </c>
+      <c r="B222" s="5">
+        <v>3.4550000000000001</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" s="4">
+        <v>43791</v>
+      </c>
+      <c r="B223" s="5">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224" s="4">
+        <v>43794</v>
+      </c>
+      <c r="B224" s="5">
+        <v>3.4609999999999999</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A225" s="4">
+        <v>43795</v>
+      </c>
+      <c r="B225" s="5">
+        <v>3.4630000000000001</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A226" s="4">
+        <v>43796</v>
+      </c>
+      <c r="B226" s="5">
+        <v>3.4710000000000001</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227" s="4">
+        <v>43797</v>
+      </c>
+      <c r="B227" s="5">
+        <v>3.4710000000000001</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228" s="4">
+        <v>43798</v>
+      </c>
+      <c r="B228" s="5">
+        <v>3.476</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A229" s="4">
+        <v>43801</v>
+      </c>
+      <c r="B229" s="5">
+        <v>3.4740000000000002</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A230" s="4">
+        <v>43802</v>
+      </c>
+      <c r="B230" s="5">
+        <v>3.4809999999999999</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231" s="4">
+        <v>43803</v>
+      </c>
+      <c r="B231" s="5">
+        <v>3.4710000000000001</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232" s="4">
+        <v>43804</v>
+      </c>
+      <c r="B232" s="5">
+        <v>3.4670000000000001</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A233" s="4">
+        <v>43805</v>
+      </c>
+      <c r="B233" s="5">
+        <v>3.4630000000000001</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A234" s="4">
+        <v>43808</v>
+      </c>
+      <c r="B234" s="5">
+        <v>3.4710000000000001</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A235" s="4">
+        <v>43809</v>
+      </c>
+      <c r="B235" s="5">
+        <v>3.4649999999999999</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A236" s="4">
+        <v>43810</v>
+      </c>
+      <c r="B236" s="5">
+        <v>3.4769999999999999</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A237" s="4">
+        <v>43811</v>
+      </c>
+      <c r="B237" s="5">
+        <v>3.4809999999999999</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A238" s="4">
+        <v>43812</v>
+      </c>
+      <c r="B238" s="5">
+        <v>3.476</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239" s="4">
+        <v>43815</v>
+      </c>
+      <c r="B239" s="5">
+        <v>3.4980000000000002</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A240" s="4">
+        <v>43816</v>
+      </c>
+      <c r="B240" s="5">
+        <v>3.492</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A241" s="4">
+        <v>43817</v>
+      </c>
+      <c r="B241" s="5">
+        <v>3.5009999999999999</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A242" s="4">
+        <v>43818</v>
+      </c>
+      <c r="B242" s="5">
+        <v>3.4929999999999999</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A243" s="4">
+        <v>43819</v>
+      </c>
+      <c r="B243" s="5">
+        <v>3.4769999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Start implementing interest support
</commit_message>
<xml_diff>
--- a/ExchangeRates.xlsx
+++ b/ExchangeRates.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105"/>
   </bookViews>
   <sheets>
-    <sheet name="ExchangeRates (4)" sheetId="1" r:id="rId1"/>
+    <sheet name="_tmp_exchanges" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -24,7 +24,7 @@
     <t>בנק ישראל - שערים יציגים</t>
   </si>
   <si>
-    <t>טווח תאריכים : 02/01/2019 - 20/12/2019</t>
+    <t>טווח תאריכים : 30/12/2018 - 31/12/2019</t>
   </si>
   <si>
     <t>אם לא פורסם שער יציג ליום המבוקש, מוצג השער האחרון שפורסם לפניו</t>
@@ -908,11 +908,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B243"/>
+  <dimension ref="A1:B250"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
-    </sheetView>
+    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -945,135 +943,135 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>43467</v>
+        <v>43465</v>
       </c>
       <c r="B6" s="5">
-        <v>3.746</v>
+        <v>3.7480000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <v>43468</v>
+        <v>43467</v>
       </c>
       <c r="B7" s="5">
-        <v>3.742</v>
+        <v>3.746</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <v>43469</v>
+        <v>43468</v>
       </c>
       <c r="B8" s="5">
-        <v>3.72</v>
+        <v>3.742</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
-        <v>43472</v>
+        <v>43469</v>
       </c>
       <c r="B9" s="5">
-        <v>3.694</v>
+        <v>3.72</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>43473</v>
+        <v>43472</v>
       </c>
       <c r="B10" s="5">
-        <v>3.6989999999999998</v>
+        <v>3.694</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <v>43474</v>
+        <v>43473</v>
       </c>
       <c r="B11" s="5">
-        <v>3.6819999999999999</v>
+        <v>3.6989999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <v>43475</v>
+        <v>43474</v>
       </c>
       <c r="B12" s="5">
-        <v>3.6640000000000001</v>
+        <v>3.6819999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <v>43476</v>
+        <v>43475</v>
       </c>
       <c r="B13" s="5">
-        <v>3.673</v>
+        <v>3.6640000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <v>43479</v>
+        <v>43476</v>
       </c>
       <c r="B14" s="5">
-        <v>3.657</v>
+        <v>3.673</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <v>43480</v>
+        <v>43479</v>
       </c>
       <c r="B15" s="5">
-        <v>3.67</v>
+        <v>3.657</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <v>43481</v>
+        <v>43480</v>
       </c>
       <c r="B16" s="5">
-        <v>3.6779999999999999</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
-        <v>43482</v>
+        <v>43481</v>
       </c>
       <c r="B17" s="5">
-        <v>3.6880000000000002</v>
+        <v>3.6779999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
-        <v>43483</v>
+        <v>43482</v>
       </c>
       <c r="B18" s="5">
-        <v>3.6920000000000002</v>
+        <v>3.6880000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
-        <v>43486</v>
+        <v>43483</v>
       </c>
       <c r="B19" s="5">
-        <v>3.698</v>
+        <v>3.6920000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>43487</v>
+        <v>43486</v>
       </c>
       <c r="B20" s="5">
-        <v>3.69</v>
+        <v>3.698</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>43488</v>
+        <v>43487</v>
       </c>
       <c r="B21" s="5">
-        <v>3.6829999999999998</v>
+        <v>3.69</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <v>43489</v>
+        <v>43488</v>
       </c>
       <c r="B22" s="5">
         <v>3.6829999999999998</v>
@@ -1081,103 +1079,103 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <v>43490</v>
+        <v>43489</v>
       </c>
       <c r="B23" s="5">
-        <v>3.6850000000000001</v>
+        <v>3.6829999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
-        <v>43493</v>
+        <v>43490</v>
       </c>
       <c r="B24" s="5">
-        <v>3.68</v>
+        <v>3.6850000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
-        <v>43494</v>
+        <v>43493</v>
       </c>
       <c r="B25" s="5">
-        <v>3.6779999999999999</v>
+        <v>3.68</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
-        <v>43495</v>
+        <v>43494</v>
       </c>
       <c r="B26" s="5">
-        <v>3.6709999999999998</v>
+        <v>3.6779999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
-        <v>43496</v>
+        <v>43495</v>
       </c>
       <c r="B27" s="5">
-        <v>3.6419999999999999</v>
+        <v>3.6709999999999998</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
-        <v>43497</v>
+        <v>43496</v>
       </c>
       <c r="B28" s="5">
-        <v>3.633</v>
+        <v>3.6419999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
-        <v>43500</v>
+        <v>43497</v>
       </c>
       <c r="B29" s="5">
-        <v>3.6269999999999998</v>
+        <v>3.633</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
-        <v>43501</v>
+        <v>43500</v>
       </c>
       <c r="B30" s="5">
-        <v>3.61</v>
+        <v>3.6269999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
-        <v>43502</v>
+        <v>43501</v>
       </c>
       <c r="B31" s="5">
-        <v>3.6190000000000002</v>
+        <v>3.61</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
-        <v>43503</v>
+        <v>43502</v>
       </c>
       <c r="B32" s="5">
-        <v>3.6269999999999998</v>
+        <v>3.6190000000000002</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
-        <v>43504</v>
+        <v>43503</v>
       </c>
       <c r="B33" s="5">
-        <v>3.6339999999999999</v>
+        <v>3.6269999999999998</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
-        <v>43507</v>
+        <v>43504</v>
       </c>
       <c r="B34" s="5">
-        <v>3.6429999999999998</v>
+        <v>3.6339999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
-        <v>43508</v>
+        <v>43507</v>
       </c>
       <c r="B35" s="5">
         <v>3.6429999999999998</v>
@@ -1185,55 +1183,55 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
-        <v>43509</v>
+        <v>43508</v>
       </c>
       <c r="B36" s="5">
-        <v>3.637</v>
+        <v>3.6429999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
-        <v>43510</v>
+        <v>43509</v>
       </c>
       <c r="B37" s="5">
-        <v>3.6619999999999999</v>
+        <v>3.637</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
-        <v>43511</v>
+        <v>43510</v>
       </c>
       <c r="B38" s="5">
-        <v>3.641</v>
+        <v>3.6619999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
-        <v>43514</v>
+        <v>43511</v>
       </c>
       <c r="B39" s="5">
-        <v>3.62</v>
+        <v>3.641</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
-        <v>43515</v>
+        <v>43514</v>
       </c>
       <c r="B40" s="5">
-        <v>3.6309999999999998</v>
+        <v>3.62</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
-        <v>43516</v>
+        <v>43515</v>
       </c>
       <c r="B41" s="5">
-        <v>3.617</v>
+        <v>3.6309999999999998</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
-        <v>43517</v>
+        <v>43516</v>
       </c>
       <c r="B42" s="5">
         <v>3.617</v>
@@ -1241,79 +1239,79 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
-        <v>43518</v>
+        <v>43517</v>
       </c>
       <c r="B43" s="5">
-        <v>3.613</v>
+        <v>3.617</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
-        <v>43521</v>
+        <v>43518</v>
       </c>
       <c r="B44" s="5">
-        <v>3.605</v>
+        <v>3.613</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
-        <v>43522</v>
+        <v>43521</v>
       </c>
       <c r="B45" s="5">
-        <v>3.6240000000000001</v>
+        <v>3.605</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
-        <v>43523</v>
+        <v>43522</v>
       </c>
       <c r="B46" s="5">
-        <v>3.6190000000000002</v>
+        <v>3.6240000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
-        <v>43524</v>
+        <v>43523</v>
       </c>
       <c r="B47" s="5">
-        <v>3.6040000000000001</v>
+        <v>3.6190000000000002</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
-        <v>43525</v>
+        <v>43524</v>
       </c>
       <c r="B48" s="5">
-        <v>3.6240000000000001</v>
+        <v>3.6040000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
-        <v>43528</v>
+        <v>43525</v>
       </c>
       <c r="B49" s="5">
-        <v>3.625</v>
+        <v>3.6240000000000001</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
-        <v>43529</v>
+        <v>43528</v>
       </c>
       <c r="B50" s="5">
-        <v>3.6190000000000002</v>
+        <v>3.625</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
-        <v>43530</v>
+        <v>43529</v>
       </c>
       <c r="B51" s="5">
-        <v>3.6160000000000001</v>
+        <v>3.6190000000000002</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
-        <v>43531</v>
+        <v>43530</v>
       </c>
       <c r="B52" s="5">
         <v>3.6160000000000001</v>
@@ -1321,463 +1319,463 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
-        <v>43532</v>
+        <v>43531</v>
       </c>
       <c r="B53" s="5">
-        <v>3.6309999999999998</v>
+        <v>3.6160000000000001</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
-        <v>43535</v>
+        <v>43532</v>
       </c>
       <c r="B54" s="5">
-        <v>3.621</v>
+        <v>3.6309999999999998</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
-        <v>43536</v>
+        <v>43535</v>
       </c>
       <c r="B55" s="5">
-        <v>3.6230000000000002</v>
+        <v>3.621</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
-        <v>43537</v>
+        <v>43536</v>
       </c>
       <c r="B56" s="5">
-        <v>3.617</v>
+        <v>3.6230000000000002</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
-        <v>43538</v>
+        <v>43537</v>
       </c>
       <c r="B57" s="5">
-        <v>3.6</v>
+        <v>3.617</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
-        <v>43539</v>
+        <v>43538</v>
       </c>
       <c r="B58" s="5">
-        <v>3.6040000000000001</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
-        <v>43542</v>
+        <v>43539</v>
       </c>
       <c r="B59" s="5">
-        <v>3.601</v>
+        <v>3.6040000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
-        <v>43543</v>
+        <v>43542</v>
       </c>
       <c r="B60" s="5">
-        <v>3.6059999999999999</v>
+        <v>3.601</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
-        <v>43544</v>
+        <v>43543</v>
       </c>
       <c r="B61" s="5">
-        <v>3.6080000000000001</v>
+        <v>3.6059999999999999</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
-        <v>43549</v>
+        <v>43544</v>
       </c>
       <c r="B62" s="5">
-        <v>3.6230000000000002</v>
+        <v>3.6080000000000001</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
-        <v>43550</v>
+        <v>43549</v>
       </c>
       <c r="B63" s="5">
-        <v>3.617</v>
+        <v>3.6230000000000002</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
-        <v>43551</v>
+        <v>43550</v>
       </c>
       <c r="B64" s="5">
-        <v>3.6349999999999998</v>
+        <v>3.617</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
-        <v>43552</v>
+        <v>43551</v>
       </c>
       <c r="B65" s="5">
-        <v>3.6360000000000001</v>
+        <v>3.6349999999999998</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
-        <v>43553</v>
+        <v>43552</v>
       </c>
       <c r="B66" s="5">
-        <v>3.6320000000000001</v>
+        <v>3.6360000000000001</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
-        <v>43556</v>
+        <v>43553</v>
       </c>
       <c r="B67" s="5">
-        <v>3.6259999999999999</v>
+        <v>3.6320000000000001</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
-        <v>43557</v>
+        <v>43556</v>
       </c>
       <c r="B68" s="5">
-        <v>3.6240000000000001</v>
+        <v>3.6259999999999999</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
-        <v>43558</v>
+        <v>43557</v>
       </c>
       <c r="B69" s="5">
-        <v>3.6</v>
+        <v>3.6240000000000001</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
-        <v>43559</v>
+        <v>43558</v>
       </c>
       <c r="B70" s="5">
-        <v>3.6030000000000002</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
-        <v>43560</v>
+        <v>43559</v>
       </c>
       <c r="B71" s="5">
-        <v>3.5870000000000002</v>
+        <v>3.6030000000000002</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
-        <v>43563</v>
+        <v>43560</v>
       </c>
       <c r="B72" s="5">
-        <v>3.58</v>
+        <v>3.5870000000000002</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
-        <v>43565</v>
+        <v>43563</v>
       </c>
       <c r="B73" s="5">
-        <v>3.5779999999999998</v>
+        <v>3.58</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
-        <v>43566</v>
+        <v>43565</v>
       </c>
       <c r="B74" s="5">
-        <v>3.5830000000000002</v>
+        <v>3.5779999999999998</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
-        <v>43567</v>
+        <v>43566</v>
       </c>
       <c r="B75" s="5">
-        <v>3.5779999999999998</v>
+        <v>3.5830000000000002</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
-        <v>43570</v>
+        <v>43567</v>
       </c>
       <c r="B76" s="5">
-        <v>3.5609999999999999</v>
+        <v>3.5779999999999998</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
-        <v>43571</v>
+        <v>43570</v>
       </c>
       <c r="B77" s="5">
-        <v>3.5579999999999998</v>
+        <v>3.5609999999999999</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
-        <v>43572</v>
+        <v>43571</v>
       </c>
       <c r="B78" s="5">
-        <v>3.5750000000000002</v>
+        <v>3.5579999999999998</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
-        <v>43573</v>
+        <v>43572</v>
       </c>
       <c r="B79" s="5">
-        <v>3.589</v>
+        <v>3.5750000000000002</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
-        <v>43578</v>
+        <v>43573</v>
       </c>
       <c r="B80" s="5">
-        <v>3.593</v>
+        <v>3.589</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
-        <v>43579</v>
+        <v>43578</v>
       </c>
       <c r="B81" s="5">
-        <v>3.6139999999999999</v>
+        <v>3.593</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
-        <v>43580</v>
+        <v>43579</v>
       </c>
       <c r="B82" s="5">
-        <v>3.6280000000000001</v>
+        <v>3.6139999999999999</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
-        <v>43584</v>
+        <v>43580</v>
       </c>
       <c r="B83" s="5">
-        <v>3.6179999999999999</v>
+        <v>3.6280000000000001</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
-        <v>43585</v>
+        <v>43584</v>
       </c>
       <c r="B84" s="5">
-        <v>3.6080000000000001</v>
+        <v>3.6179999999999999</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
-        <v>43586</v>
+        <v>43585</v>
       </c>
       <c r="B85" s="5">
-        <v>3.5859999999999999</v>
+        <v>3.6080000000000001</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
-        <v>43587</v>
+        <v>43586</v>
       </c>
       <c r="B86" s="5">
-        <v>3.5979999999999999</v>
+        <v>3.5859999999999999</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
-        <v>43588</v>
+        <v>43587</v>
       </c>
       <c r="B87" s="5">
-        <v>3.601</v>
+        <v>3.5979999999999999</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
-        <v>43591</v>
+        <v>43588</v>
       </c>
       <c r="B88" s="5">
-        <v>3.5910000000000002</v>
+        <v>3.601</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
-        <v>43592</v>
+        <v>43591</v>
       </c>
       <c r="B89" s="5">
-        <v>3.585</v>
+        <v>3.5910000000000002</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
-        <v>43593</v>
+        <v>43592</v>
       </c>
       <c r="B90" s="5">
-        <v>3.5840000000000001</v>
+        <v>3.585</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
-        <v>43595</v>
+        <v>43593</v>
       </c>
       <c r="B91" s="5">
-        <v>3.5670000000000002</v>
+        <v>3.5840000000000001</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
-        <v>43598</v>
+        <v>43595</v>
       </c>
       <c r="B92" s="5">
-        <v>3.5680000000000001</v>
+        <v>3.5670000000000002</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
-        <v>43599</v>
+        <v>43598</v>
       </c>
       <c r="B93" s="5">
-        <v>3.577</v>
+        <v>3.5680000000000001</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
-        <v>43600</v>
+        <v>43599</v>
       </c>
       <c r="B94" s="5">
-        <v>3.5710000000000002</v>
+        <v>3.577</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="4">
-        <v>43601</v>
+        <v>43600</v>
       </c>
       <c r="B95" s="5">
-        <v>3.5680000000000001</v>
+        <v>3.5710000000000002</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="4">
-        <v>43602</v>
+        <v>43601</v>
       </c>
       <c r="B96" s="5">
-        <v>3.5750000000000002</v>
+        <v>3.5680000000000001</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="4">
-        <v>43605</v>
+        <v>43602</v>
       </c>
       <c r="B97" s="5">
-        <v>3.573</v>
+        <v>3.5750000000000002</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="4">
-        <v>43606</v>
+        <v>43605</v>
       </c>
       <c r="B98" s="5">
-        <v>3.5979999999999999</v>
+        <v>3.573</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
-        <v>43607</v>
+        <v>43606</v>
       </c>
       <c r="B99" s="5">
-        <v>3.6110000000000002</v>
+        <v>3.5979999999999999</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
-        <v>43608</v>
+        <v>43607</v>
       </c>
       <c r="B100" s="5">
-        <v>3.6150000000000002</v>
+        <v>3.6110000000000002</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="4">
-        <v>43609</v>
+        <v>43608</v>
       </c>
       <c r="B101" s="5">
-        <v>3.605</v>
+        <v>3.6150000000000002</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
-        <v>43613</v>
+        <v>43609</v>
       </c>
       <c r="B102" s="5">
-        <v>3.6139999999999999</v>
+        <v>3.605</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="4">
-        <v>43614</v>
+        <v>43613</v>
       </c>
       <c r="B103" s="5">
-        <v>3.617</v>
+        <v>3.6139999999999999</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="4">
-        <v>43615</v>
+        <v>43614</v>
       </c>
       <c r="B104" s="5">
-        <v>3.62</v>
+        <v>3.617</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="4">
-        <v>43616</v>
+        <v>43615</v>
       </c>
       <c r="B105" s="5">
-        <v>3.6339999999999999</v>
+        <v>3.62</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="4">
-        <v>43619</v>
+        <v>43616</v>
       </c>
       <c r="B106" s="5">
-        <v>3.633</v>
+        <v>3.6339999999999999</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="4">
-        <v>43620</v>
+        <v>43619</v>
       </c>
       <c r="B107" s="5">
-        <v>3.6120000000000001</v>
+        <v>3.633</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="4">
-        <v>43621</v>
+        <v>43620</v>
       </c>
       <c r="B108" s="5">
-        <v>3.61</v>
+        <v>3.6120000000000001</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="4">
-        <v>43622</v>
+        <v>43621</v>
       </c>
       <c r="B109" s="5">
-        <v>3.601</v>
+        <v>3.61</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="4">
-        <v>43623</v>
+        <v>43622</v>
       </c>
       <c r="B110" s="5">
         <v>3.601</v>
@@ -1785,335 +1783,335 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
-        <v>43626</v>
+        <v>43623</v>
       </c>
       <c r="B111" s="5">
-        <v>3.585</v>
+        <v>3.601</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
-        <v>43627</v>
+        <v>43626</v>
       </c>
       <c r="B112" s="5">
-        <v>3.581</v>
+        <v>3.585</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
-        <v>43628</v>
+        <v>43627</v>
       </c>
       <c r="B113" s="5">
-        <v>3.5819999999999999</v>
+        <v>3.581</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="4">
-        <v>43629</v>
+        <v>43628</v>
       </c>
       <c r="B114" s="5">
-        <v>3.5920000000000001</v>
+        <v>3.5819999999999999</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="4">
-        <v>43630</v>
+        <v>43629</v>
       </c>
       <c r="B115" s="5">
-        <v>3.6</v>
+        <v>3.5920000000000001</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="4">
-        <v>43633</v>
+        <v>43630</v>
       </c>
       <c r="B116" s="5">
-        <v>3.61</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
-        <v>43634</v>
+        <v>43633</v>
       </c>
       <c r="B117" s="5">
-        <v>3.6120000000000001</v>
+        <v>3.61</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="4">
-        <v>43635</v>
+        <v>43634</v>
       </c>
       <c r="B118" s="5">
-        <v>3.609</v>
+        <v>3.6120000000000001</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="4">
-        <v>43636</v>
+        <v>43635</v>
       </c>
       <c r="B119" s="5">
-        <v>3.5790000000000002</v>
+        <v>3.609</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="4">
-        <v>43637</v>
+        <v>43636</v>
       </c>
       <c r="B120" s="5">
-        <v>3.5939999999999999</v>
+        <v>3.5790000000000002</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="4">
-        <v>43640</v>
+        <v>43637</v>
       </c>
       <c r="B121" s="5">
-        <v>3.6040000000000001</v>
+        <v>3.5939999999999999</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="4">
-        <v>43641</v>
+        <v>43640</v>
       </c>
       <c r="B122" s="5">
-        <v>3.6019999999999999</v>
+        <v>3.6040000000000001</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="4">
-        <v>43642</v>
+        <v>43641</v>
       </c>
       <c r="B123" s="5">
-        <v>3.5910000000000002</v>
+        <v>3.6019999999999999</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="4">
-        <v>43643</v>
+        <v>43642</v>
       </c>
       <c r="B124" s="5">
-        <v>3.5819999999999999</v>
+        <v>3.5910000000000002</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="4">
-        <v>43644</v>
+        <v>43643</v>
       </c>
       <c r="B125" s="5">
-        <v>3.5659999999999998</v>
+        <v>3.5819999999999999</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="4">
-        <v>43647</v>
+        <v>43644</v>
       </c>
       <c r="B126" s="5">
-        <v>3.5739999999999998</v>
+        <v>3.5659999999999998</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="4">
-        <v>43648</v>
+        <v>43647</v>
       </c>
       <c r="B127" s="5">
-        <v>3.5750000000000002</v>
+        <v>3.5739999999999998</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="4">
-        <v>43649</v>
+        <v>43648</v>
       </c>
       <c r="B128" s="5">
-        <v>3.5720000000000001</v>
+        <v>3.5750000000000002</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="4">
-        <v>43650</v>
+        <v>43649</v>
       </c>
       <c r="B129" s="5">
-        <v>3.5670000000000002</v>
+        <v>3.5720000000000001</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="4">
-        <v>43651</v>
+        <v>43650</v>
       </c>
       <c r="B130" s="5">
-        <v>3.5619999999999998</v>
+        <v>3.5670000000000002</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="4">
-        <v>43654</v>
+        <v>43651</v>
       </c>
       <c r="B131" s="5">
-        <v>3.573</v>
+        <v>3.5619999999999998</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="4">
-        <v>43655</v>
+        <v>43654</v>
       </c>
       <c r="B132" s="5">
-        <v>3.5680000000000001</v>
+        <v>3.573</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="4">
-        <v>43656</v>
+        <v>43655</v>
       </c>
       <c r="B133" s="5">
-        <v>3.573</v>
+        <v>3.5680000000000001</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="4">
-        <v>43657</v>
+        <v>43656</v>
       </c>
       <c r="B134" s="5">
-        <v>3.5470000000000002</v>
+        <v>3.573</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="4">
-        <v>43658</v>
+        <v>43657</v>
       </c>
       <c r="B135" s="5">
-        <v>3.5510000000000002</v>
+        <v>3.5470000000000002</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="4">
-        <v>43661</v>
+        <v>43658</v>
       </c>
       <c r="B136" s="5">
-        <v>3.5390000000000001</v>
+        <v>3.5510000000000002</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="4">
-        <v>43662</v>
+        <v>43661</v>
       </c>
       <c r="B137" s="5">
-        <v>3.5419999999999998</v>
+        <v>3.5390000000000001</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="4">
-        <v>43663</v>
+        <v>43662</v>
       </c>
       <c r="B138" s="5">
-        <v>3.5409999999999999</v>
+        <v>3.5419999999999998</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="4">
-        <v>43664</v>
+        <v>43663</v>
       </c>
       <c r="B139" s="5">
-        <v>3.5430000000000001</v>
+        <v>3.5409999999999999</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="4">
-        <v>43665</v>
+        <v>43664</v>
       </c>
       <c r="B140" s="5">
-        <v>3.5350000000000001</v>
+        <v>3.5430000000000001</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="4">
-        <v>43668</v>
+        <v>43665</v>
       </c>
       <c r="B141" s="5">
-        <v>3.5339999999999998</v>
+        <v>3.5350000000000001</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="4">
-        <v>43669</v>
+        <v>43668</v>
       </c>
       <c r="B142" s="5">
-        <v>3.5369999999999999</v>
+        <v>3.5339999999999998</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="4">
-        <v>43670</v>
+        <v>43669</v>
       </c>
       <c r="B143" s="5">
-        <v>3.5209999999999999</v>
+        <v>3.5369999999999999</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="4">
-        <v>43671</v>
+        <v>43670</v>
       </c>
       <c r="B144" s="5">
-        <v>3.5230000000000001</v>
+        <v>3.5209999999999999</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="4">
-        <v>43672</v>
+        <v>43671</v>
       </c>
       <c r="B145" s="5">
-        <v>3.5259999999999998</v>
+        <v>3.5230000000000001</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="4">
-        <v>43675</v>
+        <v>43672</v>
       </c>
       <c r="B146" s="5">
-        <v>3.5249999999999999</v>
+        <v>3.5259999999999998</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="4">
-        <v>43676</v>
+        <v>43675</v>
       </c>
       <c r="B147" s="5">
-        <v>3.5</v>
+        <v>3.5249999999999999</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="4">
-        <v>43677</v>
+        <v>43676</v>
       </c>
       <c r="B148" s="5">
-        <v>3.4990000000000001</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="4">
-        <v>43678</v>
+        <v>43677</v>
       </c>
       <c r="B149" s="5">
-        <v>3.524</v>
+        <v>3.4990000000000001</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="4">
-        <v>43679</v>
+        <v>43678</v>
       </c>
       <c r="B150" s="5">
-        <v>3.5089999999999999</v>
+        <v>3.524</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="4">
-        <v>43682</v>
+        <v>43679</v>
       </c>
       <c r="B151" s="5">
-        <v>3.4940000000000002</v>
+        <v>3.5089999999999999</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="4">
-        <v>43683</v>
+        <v>43682</v>
       </c>
       <c r="B152" s="5">
         <v>3.4940000000000002</v>
@@ -2121,599 +2119,599 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" s="4">
-        <v>43684</v>
+        <v>43683</v>
       </c>
       <c r="B153" s="5">
-        <v>3.4870000000000001</v>
+        <v>3.4940000000000002</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="4">
-        <v>43685</v>
+        <v>43684</v>
       </c>
       <c r="B154" s="5">
-        <v>3.4830000000000001</v>
+        <v>3.4870000000000001</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="4">
-        <v>43686</v>
+        <v>43685</v>
       </c>
       <c r="B155" s="5">
-        <v>3.4790000000000001</v>
+        <v>3.4830000000000001</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" s="4">
-        <v>43689</v>
+        <v>43686</v>
       </c>
       <c r="B156" s="5">
-        <v>3.484</v>
+        <v>3.4790000000000001</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="4">
-        <v>43690</v>
+        <v>43689</v>
       </c>
       <c r="B157" s="5">
-        <v>3.4929999999999999</v>
+        <v>3.484</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="4">
-        <v>43691</v>
+        <v>43690</v>
       </c>
       <c r="B158" s="5">
-        <v>3.4889999999999999</v>
+        <v>3.4929999999999999</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="4">
-        <v>43692</v>
+        <v>43691</v>
       </c>
       <c r="B159" s="5">
-        <v>3.5190000000000001</v>
+        <v>3.4889999999999999</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="4">
-        <v>43693</v>
+        <v>43692</v>
       </c>
       <c r="B160" s="5">
-        <v>3.5409999999999999</v>
+        <v>3.5190000000000001</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="4">
-        <v>43696</v>
+        <v>43693</v>
       </c>
       <c r="B161" s="5">
-        <v>3.5449999999999999</v>
+        <v>3.5409999999999999</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="4">
-        <v>43697</v>
+        <v>43696</v>
       </c>
       <c r="B162" s="5">
-        <v>3.524</v>
+        <v>3.5449999999999999</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="4">
-        <v>43698</v>
+        <v>43697</v>
       </c>
       <c r="B163" s="5">
-        <v>3.5270000000000001</v>
+        <v>3.524</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="4">
-        <v>43699</v>
+        <v>43698</v>
       </c>
       <c r="B164" s="5">
-        <v>3.5249999999999999</v>
+        <v>3.5270000000000001</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="4">
-        <v>43700</v>
+        <v>43699</v>
       </c>
       <c r="B165" s="5">
-        <v>3.5110000000000001</v>
+        <v>3.5249999999999999</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="4">
-        <v>43703</v>
+        <v>43700</v>
       </c>
       <c r="B166" s="5">
-        <v>3.5190000000000001</v>
+        <v>3.5110000000000001</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" s="4">
-        <v>43704</v>
+        <v>43703</v>
       </c>
       <c r="B167" s="5">
-        <v>3.52</v>
+        <v>3.5190000000000001</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="4">
-        <v>43705</v>
+        <v>43704</v>
       </c>
       <c r="B168" s="5">
-        <v>3.524</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" s="4">
-        <v>43706</v>
+        <v>43705</v>
       </c>
       <c r="B169" s="5">
-        <v>3.5209999999999999</v>
+        <v>3.524</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="4">
-        <v>43707</v>
+        <v>43706</v>
       </c>
       <c r="B170" s="5">
-        <v>3.5350000000000001</v>
+        <v>3.5209999999999999</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="4">
-        <v>43710</v>
+        <v>43707</v>
       </c>
       <c r="B171" s="5">
-        <v>3.5379999999999998</v>
+        <v>3.5350000000000001</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="4">
-        <v>43711</v>
+        <v>43710</v>
       </c>
       <c r="B172" s="5">
-        <v>3.5489999999999999</v>
+        <v>3.5379999999999998</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="4">
-        <v>43712</v>
+        <v>43711</v>
       </c>
       <c r="B173" s="5">
-        <v>3.5270000000000001</v>
+        <v>3.5489999999999999</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="4">
-        <v>43713</v>
+        <v>43712</v>
       </c>
       <c r="B174" s="5">
-        <v>3.512</v>
+        <v>3.5270000000000001</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" s="4">
-        <v>43714</v>
+        <v>43713</v>
       </c>
       <c r="B175" s="5">
-        <v>3.5169999999999999</v>
+        <v>3.512</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="4">
-        <v>43717</v>
+        <v>43714</v>
       </c>
       <c r="B176" s="5">
-        <v>3.5270000000000001</v>
+        <v>3.5169999999999999</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="4">
-        <v>43718</v>
+        <v>43717</v>
       </c>
       <c r="B177" s="5">
-        <v>3.5379999999999998</v>
+        <v>3.5270000000000001</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="4">
-        <v>43719</v>
+        <v>43718</v>
       </c>
       <c r="B178" s="5">
-        <v>3.544</v>
+        <v>3.5379999999999998</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="4">
-        <v>43720</v>
+        <v>43719</v>
       </c>
       <c r="B179" s="5">
-        <v>3.5409999999999999</v>
+        <v>3.544</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="4">
-        <v>43721</v>
+        <v>43720</v>
       </c>
       <c r="B180" s="5">
-        <v>3.5270000000000001</v>
+        <v>3.5409999999999999</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="4">
-        <v>43724</v>
+        <v>43721</v>
       </c>
       <c r="B181" s="5">
-        <v>3.5379999999999998</v>
+        <v>3.5270000000000001</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="4">
-        <v>43726</v>
+        <v>43724</v>
       </c>
       <c r="B182" s="5">
-        <v>3.5409999999999999</v>
+        <v>3.5379999999999998</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="4">
-        <v>43727</v>
+        <v>43726</v>
       </c>
       <c r="B183" s="5">
-        <v>3.5209999999999999</v>
+        <v>3.5409999999999999</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="4">
-        <v>43728</v>
+        <v>43727</v>
       </c>
       <c r="B184" s="5">
-        <v>3.5129999999999999</v>
+        <v>3.5209999999999999</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" s="4">
-        <v>43731</v>
+        <v>43728</v>
       </c>
       <c r="B185" s="5">
-        <v>3.5169999999999999</v>
+        <v>3.5129999999999999</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" s="4">
-        <v>43732</v>
+        <v>43731</v>
       </c>
       <c r="B186" s="5">
-        <v>3.5070000000000001</v>
+        <v>3.5169999999999999</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" s="4">
-        <v>43733</v>
+        <v>43732</v>
       </c>
       <c r="B187" s="5">
-        <v>3.5009999999999999</v>
+        <v>3.5070000000000001</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" s="4">
-        <v>43734</v>
+        <v>43733</v>
       </c>
       <c r="B188" s="5">
-        <v>3.5169999999999999</v>
+        <v>3.5009999999999999</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" s="4">
-        <v>43735</v>
+        <v>43734</v>
       </c>
       <c r="B189" s="5">
-        <v>3.4820000000000002</v>
+        <v>3.5169999999999999</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="4">
-        <v>43740</v>
+        <v>43735</v>
       </c>
       <c r="B190" s="5">
-        <v>3.4849999999999999</v>
+        <v>3.4820000000000002</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" s="4">
-        <v>43741</v>
+        <v>43740</v>
       </c>
       <c r="B191" s="5">
-        <v>3.4929999999999999</v>
+        <v>3.4849999999999999</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="4">
-        <v>43742</v>
+        <v>43741</v>
       </c>
       <c r="B192" s="5">
-        <v>3.4809999999999999</v>
+        <v>3.4929999999999999</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" s="4">
-        <v>43745</v>
+        <v>43742</v>
       </c>
       <c r="B193" s="5">
-        <v>3.4929999999999999</v>
+        <v>3.4809999999999999</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" s="4">
-        <v>43748</v>
+        <v>43745</v>
       </c>
       <c r="B194" s="5">
-        <v>3.504</v>
+        <v>3.4929999999999999</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" s="4">
-        <v>43749</v>
+        <v>43748</v>
       </c>
       <c r="B195" s="5">
-        <v>3.51</v>
+        <v>3.504</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="4">
-        <v>43753</v>
+        <v>43749</v>
       </c>
       <c r="B196" s="5">
-        <v>3.5129999999999999</v>
+        <v>3.51</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" s="4">
-        <v>43754</v>
+        <v>43753</v>
       </c>
       <c r="B197" s="5">
-        <v>3.536</v>
+        <v>3.5129999999999999</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" s="4">
-        <v>43755</v>
+        <v>43754</v>
       </c>
       <c r="B198" s="5">
-        <v>3.5449999999999999</v>
+        <v>3.536</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" s="4">
-        <v>43756</v>
+        <v>43755</v>
       </c>
       <c r="B199" s="5">
-        <v>3.5329999999999999</v>
+        <v>3.5449999999999999</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="4">
-        <v>43760</v>
+        <v>43756</v>
       </c>
       <c r="B200" s="5">
-        <v>3.5369999999999999</v>
+        <v>3.5329999999999999</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" s="4">
-        <v>43761</v>
+        <v>43760</v>
       </c>
       <c r="B201" s="5">
-        <v>3.5379999999999998</v>
+        <v>3.5369999999999999</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" s="4">
-        <v>43762</v>
+        <v>43761</v>
       </c>
       <c r="B202" s="5">
-        <v>3.5230000000000001</v>
+        <v>3.5379999999999998</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" s="4">
-        <v>43763</v>
+        <v>43762</v>
       </c>
       <c r="B203" s="5">
-        <v>3.5390000000000001</v>
+        <v>3.5230000000000001</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" s="4">
-        <v>43766</v>
+        <v>43763</v>
       </c>
       <c r="B204" s="5">
-        <v>3.5289999999999999</v>
+        <v>3.5390000000000001</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" s="4">
-        <v>43767</v>
+        <v>43766</v>
       </c>
       <c r="B205" s="5">
-        <v>3.53</v>
+        <v>3.5289999999999999</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" s="4">
-        <v>43768</v>
+        <v>43767</v>
       </c>
       <c r="B206" s="5">
-        <v>3.528</v>
+        <v>3.53</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" s="4">
-        <v>43769</v>
+        <v>43768</v>
       </c>
       <c r="B207" s="5">
-        <v>3.5289999999999999</v>
+        <v>3.528</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" s="4">
-        <v>43770</v>
+        <v>43769</v>
       </c>
       <c r="B208" s="5">
-        <v>3.5209999999999999</v>
+        <v>3.5289999999999999</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" s="4">
-        <v>43773</v>
+        <v>43770</v>
       </c>
       <c r="B209" s="5">
-        <v>3.5219999999999998</v>
+        <v>3.5209999999999999</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" s="4">
-        <v>43774</v>
+        <v>43773</v>
       </c>
       <c r="B210" s="5">
-        <v>3.5009999999999999</v>
+        <v>3.5219999999999998</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" s="4">
-        <v>43775</v>
+        <v>43774</v>
       </c>
       <c r="B211" s="5">
-        <v>3.49</v>
+        <v>3.5009999999999999</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" s="4">
-        <v>43776</v>
+        <v>43775</v>
       </c>
       <c r="B212" s="5">
-        <v>3.4870000000000001</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" s="4">
-        <v>43777</v>
+        <v>43776</v>
       </c>
       <c r="B213" s="5">
-        <v>3.4950000000000001</v>
+        <v>3.4870000000000001</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" s="4">
-        <v>43780</v>
+        <v>43777</v>
       </c>
       <c r="B214" s="5">
-        <v>3.4990000000000001</v>
+        <v>3.4950000000000001</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" s="4">
-        <v>43781</v>
+        <v>43780</v>
       </c>
       <c r="B215" s="5">
-        <v>3.5110000000000001</v>
+        <v>3.4990000000000001</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" s="4">
-        <v>43782</v>
+        <v>43781</v>
       </c>
       <c r="B216" s="5">
-        <v>3.4950000000000001</v>
+        <v>3.5110000000000001</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" s="4">
-        <v>43783</v>
+        <v>43782</v>
       </c>
       <c r="B217" s="5">
-        <v>3.488</v>
+        <v>3.4950000000000001</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" s="4">
-        <v>43784</v>
+        <v>43783</v>
       </c>
       <c r="B218" s="5">
-        <v>3.4780000000000002</v>
+        <v>3.488</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" s="4">
-        <v>43787</v>
+        <v>43784</v>
       </c>
       <c r="B219" s="5">
-        <v>3.4630000000000001</v>
+        <v>3.4780000000000002</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" s="4">
-        <v>43788</v>
+        <v>43787</v>
       </c>
       <c r="B220" s="5">
-        <v>3.4569999999999999</v>
+        <v>3.4630000000000001</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" s="4">
-        <v>43789</v>
+        <v>43788</v>
       </c>
       <c r="B221" s="5">
-        <v>3.4710000000000001</v>
+        <v>3.4569999999999999</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" s="4">
-        <v>43790</v>
+        <v>43789</v>
       </c>
       <c r="B222" s="5">
-        <v>3.4550000000000001</v>
+        <v>3.4710000000000001</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" s="4">
-        <v>43791</v>
+        <v>43790</v>
       </c>
       <c r="B223" s="5">
-        <v>3.46</v>
+        <v>3.4550000000000001</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" s="4">
-        <v>43794</v>
+        <v>43791</v>
       </c>
       <c r="B224" s="5">
-        <v>3.4609999999999999</v>
+        <v>3.46</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" s="4">
-        <v>43795</v>
+        <v>43794</v>
       </c>
       <c r="B225" s="5">
-        <v>3.4630000000000001</v>
+        <v>3.4609999999999999</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" s="4">
-        <v>43796</v>
+        <v>43795</v>
       </c>
       <c r="B226" s="5">
-        <v>3.4710000000000001</v>
+        <v>3.4630000000000001</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" s="4">
-        <v>43797</v>
+        <v>43796</v>
       </c>
       <c r="B227" s="5">
         <v>3.4710000000000001</v>
@@ -2721,130 +2719,186 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" s="4">
-        <v>43798</v>
+        <v>43797</v>
       </c>
       <c r="B228" s="5">
-        <v>3.476</v>
+        <v>3.4710000000000001</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" s="4">
-        <v>43801</v>
+        <v>43798</v>
       </c>
       <c r="B229" s="5">
-        <v>3.4740000000000002</v>
+        <v>3.476</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" s="4">
-        <v>43802</v>
+        <v>43801</v>
       </c>
       <c r="B230" s="5">
-        <v>3.4809999999999999</v>
+        <v>3.4740000000000002</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" s="4">
-        <v>43803</v>
+        <v>43802</v>
       </c>
       <c r="B231" s="5">
-        <v>3.4710000000000001</v>
+        <v>3.4809999999999999</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" s="4">
-        <v>43804</v>
+        <v>43803</v>
       </c>
       <c r="B232" s="5">
-        <v>3.4670000000000001</v>
+        <v>3.4710000000000001</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" s="4">
-        <v>43805</v>
+        <v>43804</v>
       </c>
       <c r="B233" s="5">
-        <v>3.4630000000000001</v>
+        <v>3.4670000000000001</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" s="4">
-        <v>43808</v>
+        <v>43805</v>
       </c>
       <c r="B234" s="5">
-        <v>3.4710000000000001</v>
+        <v>3.4630000000000001</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" s="4">
-        <v>43809</v>
+        <v>43808</v>
       </c>
       <c r="B235" s="5">
-        <v>3.4649999999999999</v>
+        <v>3.4710000000000001</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" s="4">
-        <v>43810</v>
+        <v>43809</v>
       </c>
       <c r="B236" s="5">
-        <v>3.4769999999999999</v>
+        <v>3.4649999999999999</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" s="4">
-        <v>43811</v>
+        <v>43810</v>
       </c>
       <c r="B237" s="5">
-        <v>3.4809999999999999</v>
+        <v>3.4769999999999999</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" s="4">
-        <v>43812</v>
+        <v>43811</v>
       </c>
       <c r="B238" s="5">
-        <v>3.476</v>
+        <v>3.4809999999999999</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" s="4">
-        <v>43815</v>
+        <v>43812</v>
       </c>
       <c r="B239" s="5">
-        <v>3.4980000000000002</v>
+        <v>3.476</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" s="4">
-        <v>43816</v>
+        <v>43815</v>
       </c>
       <c r="B240" s="5">
-        <v>3.492</v>
+        <v>3.4980000000000002</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" s="4">
-        <v>43817</v>
+        <v>43816</v>
       </c>
       <c r="B241" s="5">
-        <v>3.5009999999999999</v>
+        <v>3.492</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" s="4">
-        <v>43818</v>
+        <v>43817</v>
       </c>
       <c r="B242" s="5">
-        <v>3.4929999999999999</v>
+        <v>3.5009999999999999</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" s="4">
+        <v>43818</v>
+      </c>
+      <c r="B243" s="5">
+        <v>3.4929999999999999</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A244" s="4">
         <v>43819</v>
       </c>
-      <c r="B243" s="5">
+      <c r="B244" s="5">
         <v>3.4769999999999999</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A245" s="4">
+        <v>43822</v>
+      </c>
+      <c r="B245" s="5">
+        <v>3.472</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A246" s="4">
+        <v>43823</v>
+      </c>
+      <c r="B246" s="5">
+        <v>3.4660000000000002</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A247" s="4">
+        <v>43825</v>
+      </c>
+      <c r="B247" s="5">
+        <v>3.472</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A248" s="4">
+        <v>43826</v>
+      </c>
+      <c r="B248" s="5">
+        <v>3.468</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A249" s="4">
+        <v>43829</v>
+      </c>
+      <c r="B249" s="5">
+        <v>3.4630000000000001</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A250" s="4">
+        <v>43830</v>
+      </c>
+      <c r="B250" s="5">
+        <v>3.456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>